<commit_message>
delete and update users
</commit_message>
<xml_diff>
--- a/public/Pilot Users.xlsx
+++ b/public/Pilot Users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashbeemorgado/devs/laf/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA78FB7C-D135-F24A-BB9F-17ED276989A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BD6E65-CDC1-8F40-AE38-88BAF810631B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="500" windowWidth="24860" windowHeight="20740" xr2:uid="{14EFB9D0-AEA6-1448-9800-D24928032668}"/>
   </bookViews>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B009895-59D4-354B-A067-D2137EB65BC7}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>